<commit_message>
Replaced tag svgs with html components (Fixed #11)
</commit_message>
<xml_diff>
--- a/src/data/tag_info.xlsx
+++ b/src/data/tag_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\twin_shelves_2\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6DFC7F-2489-4CFD-A4F5-873D2A111150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3D4D86-5D24-4C6F-8C51-6A28E1A10132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{B2B09A5B-CDA6-4ED8-82F1-5DF6C662589A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{B2B09A5B-CDA6-4ED8-82F1-5DF6C662589A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>topic_1</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>spacer_height</t>
+  </si>
+  <si>
+    <t>number_of_bars</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -296,7 +299,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -636,22 +639,22 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="I26" sqref="A1:I26"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1796875" customWidth="1"/>
-    <col min="8" max="8" width="3.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -679,6 +682,9 @@
       <c r="I1" t="s">
         <v>59</v>
       </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
       <c r="N1" t="s">
         <v>60</v>
       </c>
@@ -686,7 +692,7 @@
         <v>8.5180000000000007</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -700,14 +706,14 @@
         <v>430</v>
       </c>
       <c r="E2" s="3">
-        <f>C2/D2</f>
+        <f t="shared" ref="E2:E26" si="0">C2/D2</f>
         <v>0.1032093023255814</v>
       </c>
       <c r="F2" s="4">
         <v>70.754999999999995</v>
       </c>
       <c r="G2" s="3">
-        <f>F2/D2</f>
+        <f t="shared" ref="G2:G26" si="1">F2/D2</f>
         <v>0.16454651162790696</v>
       </c>
       <c r="H2" s="5">
@@ -717,6 +723,9 @@
         <f>(3+(H2-1)*($O$1+$O$3))/(48.732+5)</f>
         <v>5.5832650934266356E-2</v>
       </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
       <c r="N2" t="s">
         <v>13</v>
       </c>
@@ -724,7 +733,7 @@
         <v>3.9689999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -738,7 +747,7 @@
         <v>430</v>
       </c>
       <c r="E3" s="3">
-        <f>C3/D3</f>
+        <f t="shared" si="0"/>
         <v>0.19801387688578606</v>
       </c>
       <c r="F3" s="4">
@@ -746,15 +755,18 @@
         <v>119.10399999999998</v>
       </c>
       <c r="G3" s="3">
-        <f>F3/D3</f>
+        <f t="shared" si="1"/>
         <v>0.27698604651162789</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
       </c>
       <c r="I3" s="7">
-        <f t="shared" ref="I3:I26" si="0">(3+(H3-1)*($O$1+$O$3))/(48.732+5)</f>
+        <f t="shared" ref="I3:I26" si="2">(3+(H3-1)*($O$1+$O$3))/(48.732+5)</f>
         <v>5.5832650934266356E-2</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
       </c>
       <c r="N3" t="s">
         <v>62</v>
@@ -763,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -777,7 +789,7 @@
         <v>430</v>
       </c>
       <c r="E4" s="3">
-        <f>C4/D4</f>
+        <f t="shared" si="0"/>
         <v>9.3725449019958759E-2</v>
       </c>
       <c r="F4" s="4">
@@ -785,18 +797,21 @@
         <v>208.21896706088799</v>
       </c>
       <c r="G4" s="3">
-        <f>F4/D4</f>
+        <f t="shared" si="1"/>
         <v>0.48423015595555347</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
       </c>
       <c r="I4" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.5832650934266356E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -810,7 +825,7 @@
         <v>430</v>
       </c>
       <c r="E5" s="3">
-        <f>C5/D5</f>
+        <f t="shared" si="0"/>
         <v>5.5580625072000907E-2</v>
       </c>
       <c r="F5" s="4">
@@ -818,18 +833,21 @@
         <v>252.48991013947025</v>
       </c>
       <c r="G5" s="3">
-        <f>F5/D5</f>
+        <f t="shared" si="1"/>
         <v>0.58718583753365172</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
       </c>
       <c r="I5" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.5832650934266356E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -843,7 +861,7 @@
         <v>430</v>
       </c>
       <c r="E6" s="3">
-        <f>C6/D6</f>
+        <f t="shared" si="0"/>
         <v>0.10372245293213191</v>
       </c>
       <c r="F6" s="4">
@@ -851,19 +869,22 @@
         <v>280.35857892043066</v>
       </c>
       <c r="G6" s="3">
-        <f>F6/D6</f>
+        <f t="shared" si="1"/>
         <v>0.65199669516379222</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
       </c>
       <c r="I6" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.5832650934266356E-2</v>
       </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -877,7 +898,7 @@
         <v>430</v>
       </c>
       <c r="E7" s="3">
-        <f>C7/D7</f>
+        <f t="shared" si="0"/>
         <v>7.9213851720008624E-2</v>
       </c>
       <c r="F7" s="4">
@@ -885,18 +906,21 @@
         <v>328.92823368124738</v>
       </c>
       <c r="G7" s="3">
-        <f>F7/D7</f>
+        <f t="shared" si="1"/>
         <v>0.7649493806540637</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
       </c>
       <c r="I7" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.5832650934266356E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -910,25 +934,28 @@
         <v>430</v>
       </c>
       <c r="E8" s="3">
-        <f>C8/D8</f>
+        <f t="shared" si="0"/>
         <v>9.5961050008055618E-2</v>
       </c>
       <c r="F8">
         <v>86.338999999999999</v>
       </c>
       <c r="G8" s="3">
-        <f>F8/D8</f>
+        <f t="shared" si="1"/>
         <v>0.20078837209302325</v>
       </c>
       <c r="H8" s="5">
         <v>2</v>
       </c>
       <c r="I8" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23297104146504877</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -942,7 +969,7 @@
         <v>430</v>
       </c>
       <c r="E9" s="3">
-        <f>C9/D9</f>
+        <f t="shared" si="0"/>
         <v>0.10095106234013675</v>
       </c>
       <c r="F9" s="4">
@@ -950,18 +977,21 @@
         <v>131.57125150346391</v>
       </c>
       <c r="G9" s="3">
-        <f>F9/D9</f>
+        <f t="shared" si="1"/>
         <v>0.30597965465921839</v>
       </c>
       <c r="H9" s="5">
         <v>2</v>
       </c>
       <c r="I9" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23297104146504877</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -975,26 +1005,29 @@
         <v>430</v>
       </c>
       <c r="E10" s="3">
-        <f>C10/D10</f>
+        <f t="shared" si="0"/>
         <v>8.7543116160892637E-2</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" ref="F10:F13" si="1">F9+C9+$O$2</f>
+        <f t="shared" ref="F10:F13" si="3">F9+C9+$O$2</f>
         <v>178.94920830972271</v>
       </c>
       <c r="G10" s="3">
-        <f>F10/D10</f>
+        <f t="shared" si="1"/>
         <v>0.41616094955749466</v>
       </c>
       <c r="H10" s="5">
         <v>2</v>
       </c>
       <c r="I10" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23297104146504877</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1008,26 +1041,29 @@
         <v>430</v>
       </c>
       <c r="E11" s="3">
-        <f>C11/D11</f>
+        <f t="shared" si="0"/>
         <v>9.5013985285671954E-2</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>220.56174825890653</v>
       </c>
       <c r="G11" s="3">
-        <f>F11/D11</f>
+        <f t="shared" si="1"/>
         <v>0.51293429827652681</v>
       </c>
       <c r="H11" s="5">
         <v>2</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23297104146504877</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1041,26 +1077,29 @@
         <v>430</v>
       </c>
       <c r="E12" s="3">
-        <f>C12/D12</f>
+        <f t="shared" si="0"/>
         <v>0.11293086510335611</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>265.38676193174547</v>
       </c>
       <c r="G12" s="3">
-        <f>F12/D12</f>
+        <f t="shared" si="1"/>
         <v>0.61717851612033825</v>
       </c>
       <c r="H12" s="5">
         <v>2</v>
       </c>
       <c r="I12" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23297104146504877</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1074,26 +1113,29 @@
         <v>430</v>
       </c>
       <c r="E13" s="3">
-        <f>C13/D13</f>
+        <f t="shared" si="0"/>
         <v>6.8575409549647359E-2</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>317.91603392618862</v>
       </c>
       <c r="G13" s="3">
-        <f>F13/D13</f>
+        <f t="shared" si="1"/>
         <v>0.73933961378183399</v>
       </c>
       <c r="H13" s="5">
         <v>2</v>
       </c>
       <c r="I13" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23297104146504877</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1107,25 +1149,28 @@
         <v>430</v>
       </c>
       <c r="E14" s="3">
-        <f>C14/D14</f>
+        <f t="shared" si="0"/>
         <v>0.15312451831129131</v>
       </c>
       <c r="F14">
         <v>75.816999999999993</v>
       </c>
       <c r="G14" s="3">
-        <f>F14/D14</f>
+        <f t="shared" si="1"/>
         <v>0.17631860465116278</v>
       </c>
       <c r="H14" s="5">
         <v>3</v>
       </c>
       <c r="I14" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.41010943199583122</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1139,7 +1184,7 @@
         <v>430</v>
       </c>
       <c r="E15" s="3">
-        <f>C15/D15</f>
+        <f t="shared" si="0"/>
         <v>4.9607702938402089E-2</v>
       </c>
       <c r="F15" s="4">
@@ -1147,18 +1192,21 @@
         <v>145.62954287385526</v>
       </c>
       <c r="G15" s="3">
-        <f>F15/D15</f>
+        <f t="shared" si="1"/>
         <v>0.33867335552059363</v>
       </c>
       <c r="H15" s="5">
         <v>3</v>
       </c>
       <c r="I15" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.41010943199583122</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1172,26 +1220,29 @@
         <v>430</v>
       </c>
       <c r="E16" s="3">
-        <f>C16/D16</f>
+        <f t="shared" si="0"/>
         <v>7.3050384692065679E-2</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F16:F19" si="2">F15+C15+$O$2</f>
+        <f t="shared" ref="F16:F19" si="4">F15+C15+$O$2</f>
         <v>170.92985513736815</v>
       </c>
       <c r="G16" s="3">
-        <f>F16/D16</f>
+        <f t="shared" si="1"/>
         <v>0.39751129101713523</v>
       </c>
       <c r="H16" s="5">
         <v>3</v>
       </c>
       <c r="I16" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.41010943199583122</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1205,26 +1256,29 @@
         <v>430</v>
       </c>
       <c r="E17" s="3">
-        <f>C17/D17</f>
+        <f t="shared" si="0"/>
         <v>0.10351681537288923</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>206.31052055495638</v>
       </c>
       <c r="G17" s="3">
-        <f>F17/D17</f>
+        <f t="shared" si="1"/>
         <v>0.47979190826734042</v>
       </c>
       <c r="H17" s="5">
         <v>3</v>
       </c>
       <c r="I17" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.41010943199583122</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1238,26 +1292,29 @@
         <v>430</v>
       </c>
       <c r="E18" s="3">
-        <f>C18/D18</f>
+        <f t="shared" si="0"/>
         <v>0.11542681456095284</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>254.79175116529876</v>
       </c>
       <c r="G18" s="3">
-        <f>F18/D18</f>
+        <f t="shared" si="1"/>
         <v>0.59253895619836927</v>
       </c>
       <c r="H18" s="5">
         <v>3</v>
       </c>
       <c r="I18" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.41010943199583122</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1271,26 +1328,29 @@
         <v>430</v>
       </c>
       <c r="E19" s="3">
-        <f>C19/D19</f>
+        <f t="shared" si="0"/>
         <v>0.11518910508880077</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>308.39428142650848</v>
       </c>
       <c r="G19" s="3">
-        <f>F19/D19</f>
+        <f t="shared" si="1"/>
         <v>0.71719600331746158</v>
       </c>
       <c r="H19" s="5">
         <v>3</v>
       </c>
       <c r="I19" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.41010943199583122</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1304,25 +1364,28 @@
         <v>430</v>
       </c>
       <c r="E20" s="3">
-        <f>C20/D20</f>
+        <f t="shared" si="0"/>
         <v>8.5047166703295901E-2</v>
       </c>
       <c r="F20">
         <v>60.189</v>
       </c>
       <c r="G20" s="3">
-        <f>F20/D20</f>
+        <f t="shared" si="1"/>
         <v>0.13997441860465115</v>
       </c>
       <c r="H20" s="5">
         <v>4</v>
       </c>
       <c r="I20" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.58724782252661356</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1336,7 +1399,7 @@
         <v>430</v>
       </c>
       <c r="E21" s="3">
-        <f>C21/D21</f>
+        <f t="shared" si="0"/>
         <v>9.9215405876804177E-2</v>
       </c>
       <c r="F21" s="4">
@@ -1344,18 +1407,21 @@
         <v>100.72828168241723</v>
       </c>
       <c r="G21" s="3">
-        <f>F21/D21</f>
+        <f t="shared" si="1"/>
         <v>0.23425181786608659</v>
       </c>
       <c r="H21" s="5">
         <v>4</v>
       </c>
       <c r="I21" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.58724782252661356</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1369,26 +1435,29 @@
         <v>430</v>
       </c>
       <c r="E22" s="3">
-        <f>C22/D22</f>
+        <f t="shared" si="0"/>
         <v>0.10234713384325206</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" ref="F22:F26" si="3">F21+C21+$O$2</f>
+        <f t="shared" ref="F22:F26" si="5">F21+C21+$O$2</f>
         <v>147.35990620944301</v>
       </c>
       <c r="G22" s="3">
-        <f>F22/D22</f>
+        <f t="shared" si="1"/>
         <v>0.34269745630103027</v>
       </c>
       <c r="H22" s="5">
         <v>4</v>
       </c>
       <c r="I22" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.58724782252661356</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1402,26 +1471,29 @@
         <v>430</v>
       </c>
       <c r="E23" s="3">
-        <f>C23/D23</f>
+        <f t="shared" si="0"/>
         <v>0.11048773997290427</v>
       </c>
       <c r="F23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>195.33817376204138</v>
       </c>
       <c r="G23" s="3">
-        <f>F23/D23</f>
+        <f t="shared" si="1"/>
         <v>0.45427482270242181</v>
       </c>
       <c r="H23" s="5">
         <v>4</v>
       </c>
       <c r="I23" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.58724782252661356</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1435,26 +1507,29 @@
         <v>430</v>
       </c>
       <c r="E24" s="3">
-        <f>C24/D24</f>
+        <f t="shared" si="0"/>
         <v>0.10845966312716243</v>
       </c>
       <c r="F24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>246.81690195039022</v>
       </c>
       <c r="G24" s="3">
-        <f>F24/D24</f>
+        <f t="shared" si="1"/>
         <v>0.57399279523346558</v>
       </c>
       <c r="H24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.58724782252661356</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1468,26 +1543,29 @@
         <v>430</v>
       </c>
       <c r="E25" s="3">
-        <f>C25/D25</f>
+        <f t="shared" si="0"/>
         <v>8.6028189921701276E-2</v>
       </c>
       <c r="F25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>297.42355709507007</v>
       </c>
       <c r="G25" s="3">
-        <f>F25/D25</f>
+        <f t="shared" si="1"/>
         <v>0.69168269091876755</v>
       </c>
       <c r="H25" s="5">
         <v>4</v>
       </c>
       <c r="I25" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.58724782252661356</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1501,26 +1579,29 @@
         <v>430</v>
       </c>
       <c r="E26" s="3">
-        <f>C26/D26</f>
+        <f t="shared" si="0"/>
         <v>8.3532240464104554E-2</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>338.38467876140163</v>
       </c>
       <c r="G26" s="3">
-        <f>F26/D26</f>
+        <f t="shared" si="1"/>
         <v>0.78694111339860839</v>
       </c>
       <c r="H26" s="5">
         <v>4</v>
       </c>
       <c r="I26" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.58724782252661356</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>20</v>
       </c>

</xml_diff>